<commit_message>
Fix overflow calculations (SHEET-52)
Change-Id: I0dbc58ad8d92abba974b9b64bbcbd16058763775
</commit_message>
<xml_diff>
--- a/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet/src/test/resources/test_sheets/column_alignment_style.xlsx
+++ b/vaadin-spreadsheet-flow-parent/vaadin-spreadsheet/src/test/resources/test_sheets/column_alignment_style.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25725"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26004"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="31940" yWindow="4580" windowWidth="24860" windowHeight="16720" tabRatio="500"/>
@@ -18,9 +18,23 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Local Total</t>
+  </si>
+  <si>
+    <t>Long header (Loooooong)</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -39,6 +53,22 @@
       <color rgb="FF1F497D"/>
       <name val="Tahoma"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -54,7 +84,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -71,11 +101,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0"/>
+      </left>
+      <right style="thin">
+        <color theme="0"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -83,8 +128,22 @@
     <xf numFmtId="3" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,15 +473,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="14.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -430,7 +492,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -438,8 +500,26 @@
         <v>4</v>
       </c>
     </row>
+    <row r="4" spans="1:4" ht="42" customHeight="1">
+      <c r="D4" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="22" customHeight="1">
+      <c r="D5" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="55" customHeight="1" thickBot="1">
+      <c r="A6" s="3"/>
+      <c r="D6" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="16" thickTop="1"/>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>